<commit_message>
added new method, updated Test steps , Updated Excel Data
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/approvalProcess.xlsx
+++ b/src/test/resources/datasheets/approvalProcess.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19635" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="FinanceApprover" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>XEEVA -MJ</t>
   </si>
   <si>
-    <t>REPOFLOR 100 MG</t>
-  </si>
-  <si>
     <t>UNSPSC001</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>Supplier</t>
+  </si>
+  <si>
+    <t>DESKTOP</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -552,31 +552,31 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
       <c r="P1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
-        <v>33</v>
-      </c>
       <c r="S1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" t="s">
-        <v>39</v>
-      </c>
       <c r="V1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -587,64 +587,64 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
       <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" t="s">
-        <v>35</v>
-      </c>
       <c r="S2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="U2" t="s">
-        <v>41</v>
-      </c>
       <c r="V2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>